<commit_message>
update with multiple work sheets
</commit_message>
<xml_diff>
--- a/etlcsvmongodb/uploads/test.xlsx
+++ b/etlcsvmongodb/uploads/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="District GAPS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>SD Code</t>
   </si>
@@ -96,45 +96,6 @@
   </si>
   <si>
     <t>Oti East</t>
-  </si>
-  <si>
-    <t>OTI-S-0002</t>
-  </si>
-  <si>
-    <t>Krachi West</t>
-  </si>
-  <si>
-    <t>Ehiamankyene (Krachi West)</t>
-  </si>
-  <si>
-    <t>Ehiamankyene</t>
-  </si>
-  <si>
-    <t>Krachi West in bracket attached in DHIMs</t>
-  </si>
-  <si>
-    <t>OTI-S-0003</t>
-  </si>
-  <si>
-    <t>Island(Krachi West)</t>
-  </si>
-  <si>
-    <t>Island (Krachi West)</t>
-  </si>
-  <si>
-    <t>There's a space in between the Island and the bracket in the DHIMs</t>
-  </si>
-  <si>
-    <t>OTI-S-0004</t>
-  </si>
-  <si>
-    <t>Chayo</t>
-  </si>
-  <si>
-    <t>Gyato Chayo</t>
-  </si>
-  <si>
-    <t>DHIMs did not have Gyato attached to Chayo</t>
   </si>
   <si>
     <t>Sub-District</t>
@@ -615,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -684,10 +645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -772,75 +733,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="6" customFormat="1" ht="15.6">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" s="6" customFormat="1" ht="15.6">
-      <c r="A4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" s="6" customFormat="1" ht="15.6">
-      <c r="A5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -850,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -877,19 +769,19 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>17</v>
@@ -897,57 +789,57 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>